<commit_message>
add associatedReferences column in the synonyms sheet
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="accepted names" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t xml:space="preserve">namecode</t>
   </si>
@@ -65,6 +65,7 @@
       <sz val="10"/>
       <name val="PingFang TC"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,7 +159,7 @@
   </sheetPr>
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
@@ -217,12 +219,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -232,8 +234,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,13 +256,16 @@
         <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>